<commit_message>
Added ticks & fixed France
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -30997,11 +30997,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="426724680"/>
-        <c:axId val="426724288"/>
+        <c:axId val="262936256"/>
+        <c:axId val="262940568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426724680"/>
+        <c:axId val="262936256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -31044,7 +31044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426724288"/>
+        <c:crossAx val="262940568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -31052,7 +31052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426724288"/>
+        <c:axId val="262940568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -31103,7 +31103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426724680"/>
+        <c:crossAx val="262936256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -32040,8 +32040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I628"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I601" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="R611" sqref="R611"/>
+    <sheetView tabSelected="1" topLeftCell="A592" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F530" sqref="F530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>